<commit_message>
Añadida carpeta Fase 3
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Complementos EDT.xlsx
+++ b/Fase 2/Evidencias Proyecto/Complementos EDT.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="hElpQsOtWxBvsRMwBWiilTMNcUqVEr+Yl4wHb6K5DVQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="xMvN9ienHkYj1KCIFlyjDnUV7Z0Ah8mWrWzb7Isdsyo="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>Código EDT</t>
   </si>
@@ -198,7 +198,7 @@
     <t>1.4.1.6</t>
   </si>
   <si>
-    <t>Crear vista Inventario</t>
+    <t>Crear vista Insumos</t>
   </si>
   <si>
     <t>1.4.1.7</t>
@@ -210,43 +210,61 @@
     <t>1.4.1.8</t>
   </si>
   <si>
+    <t>Crear vista Modificación Insumo</t>
+  </si>
+  <si>
+    <t>1.4.1.9</t>
+  </si>
+  <si>
     <t>Integrar navegación entre vistas</t>
   </si>
   <si>
-    <t>1.4.1.9</t>
+    <t>1.4.1.10</t>
   </si>
   <si>
     <t>Crear formulario Vehículos</t>
   </si>
   <si>
-    <t>1.4.1.10</t>
+    <t>1.4.1.11</t>
   </si>
   <si>
     <t>Crear formulario Inventario</t>
   </si>
   <si>
-    <t>1.4.1.11</t>
+    <t>1.4.1.12</t>
   </si>
   <si>
     <t>Crear formulario Mantenciones</t>
   </si>
   <si>
-    <t>1.4.1.12</t>
+    <t>1.4.1.13</t>
+  </si>
+  <si>
+    <t>Crear formulario Modificación Insumo</t>
+  </si>
+  <si>
+    <t>1.4.1.14</t>
   </si>
   <si>
     <t>Integrar operaciones CRUD Vehículo</t>
   </si>
   <si>
-    <t>1.4.1.13</t>
+    <t>1.4.1.15</t>
   </si>
   <si>
     <t>Integrar operaciones CRUD Inventario</t>
   </si>
   <si>
-    <t>1.4.1.14</t>
+    <t>1.4.1.16</t>
   </si>
   <si>
     <t>Integrar operaciones CRUD Mantención</t>
+  </si>
+  <si>
+    <t>1.4.1.17</t>
+  </si>
+  <si>
+    <t>Integrar operaciones CRUD Modificación Insumo</t>
   </si>
   <si>
     <t>1.4.2.</t>
@@ -1329,17 +1347,17 @@
       <c r="T32" s="20"/>
       <c r="U32" s="20"/>
     </row>
-    <row r="33" ht="15.0" customHeight="1" outlineLevel="1">
-      <c r="A33" s="17" t="s">
+    <row r="33" ht="15.75" customHeight="1" outlineLevel="1">
+      <c r="A33" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="19"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
@@ -1356,7 +1374,7 @@
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
     </row>
-    <row r="34" ht="15.0" customHeight="1" outlineLevel="1">
+    <row r="34" ht="15.75" customHeight="1" outlineLevel="1">
       <c r="A34" s="21" t="s">
         <v>79</v>
       </c>
@@ -1366,9 +1384,7 @@
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="13"/>
-      <c r="F34" s="19" t="s">
-        <v>81</v>
-      </c>
+      <c r="F34" s="20"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
@@ -1385,19 +1401,17 @@
       <c r="T34" s="20"/>
       <c r="U34" s="20"/>
     </row>
-    <row r="35" ht="15.0" customHeight="1" outlineLevel="1">
+    <row r="35" ht="15.75" customHeight="1" outlineLevel="1">
       <c r="A35" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="19" t="s">
-        <v>84</v>
-      </c>
+      <c r="F35" s="20"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
@@ -1414,47 +1428,123 @@
       <c r="T35" s="20"/>
       <c r="U35" s="20"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="7" t="s">
+    <row r="36" ht="15.0" customHeight="1" outlineLevel="1">
+      <c r="A36" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+    </row>
+    <row r="37" ht="15.0" customHeight="1" outlineLevel="1">
+      <c r="A37" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+    </row>
+    <row r="38" ht="15.0" customHeight="1" outlineLevel="1">
+      <c r="A38" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" outlineLevel="1">
-      <c r="A37" s="11" t="s">
+      <c r="B39" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" outlineLevel="1">
+      <c r="A40" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1" outlineLevel="1">
-      <c r="A38" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="16"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="23"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="23"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="23"/>
+      <c r="B40" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1" outlineLevel="1">
+      <c r="A41" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="16"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="23"/>
@@ -2035,9 +2125,15 @@
     <row r="234" ht="15.75" customHeight="1">
       <c r="A234" s="23"/>
     </row>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1">
+      <c r="A235" s="23"/>
+    </row>
+    <row r="236" ht="15.75" customHeight="1">
+      <c r="A236" s="23"/>
+    </row>
+    <row r="237" ht="15.75" customHeight="1">
+      <c r="A237" s="23"/>
+    </row>
     <row r="238" ht="15.75" customHeight="1"/>
     <row r="239" ht="15.75" customHeight="1"/>
     <row r="240" ht="15.75" customHeight="1"/>
@@ -2745,10 +2841,13 @@
     <row r="942" ht="15.75" customHeight="1"/>
     <row r="943" ht="15.75" customHeight="1"/>
     <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E3:E16"/>
-    <mergeCell ref="E17:E38"/>
+    <mergeCell ref="E17:E41"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>